<commit_message>
Division method for diferences
</commit_message>
<xml_diff>
--- a/2. Suma de enteros base DOS/SD-MTDeterminista1C.xlsx
+++ b/2. Suma de enteros base DOS/SD-MTDeterminista1C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34630\OneDrive\Escritorio\Universidad\4º\2º Cuatrimestre\TAC\P2MT\Practica_MT_TAC\2. Suma de enteros base DOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7555CCD-79B2-4331-BBAE-8D8C5304B09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E697D-F748-4D9D-B97D-833A3B602A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F9F779F-0B5B-4B52-81CD-964E4560136B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t xml:space="preserve">  PASOS</t>
   </si>
@@ -68,6 +68,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,6 +194,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -378,7 +385,7 @@
                   <c:v>12317</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57379</c:v>
+                  <c:v>26656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,7 +460,7 @@
                   <c:v>6659</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45062</c:v>
+                  <c:v>14339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -525,7 +532,7 @@
                   <c:v>3584</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38403</c:v>
+                  <c:v>7680</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,7 +601,7 @@
                   <c:v>1920</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34819</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,14 +1364,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>782954</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>65721</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>73341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>742949</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>55244</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1689,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A09BB4A-54DC-429E-B086-C294D4F51FFD}">
-  <dimension ref="B2:AA11"/>
+  <dimension ref="B2:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,7 +1817,7 @@
         <v>12317</v>
       </c>
       <c r="L4" s="1">
-        <v>57379</v>
+        <v>26656</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1867,7 +1874,7 @@
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L11" si="3">L4-K4</f>
-        <v>45062</v>
+        <v>14339</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1921,7 +1928,7 @@
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>38403</v>
+        <v>7680</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1972,7 +1979,7 @@
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>34819</v>
+        <v>4096</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -2020,7 +2027,7 @@
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>32899</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.3">
@@ -2050,7 +2057,7 @@
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>31875</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.3">
@@ -2077,7 +2084,7 @@
       </c>
       <c r="L10" s="1">
         <f t="shared" si="3"/>
-        <v>31331</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.3">
@@ -2101,8 +2108,308 @@
       </c>
       <c r="L11" s="7">
         <f t="shared" si="3"/>
-        <v>31043</v>
-      </c>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>6</v>
+      </c>
+      <c r="I14" s="3">
+        <v>7</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8</v>
+      </c>
+      <c r="K14" s="1">
+        <v>9</v>
+      </c>
+      <c r="L14" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9">
+        <f>D4/C4</f>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" ref="E15:L15" si="6">E4/D4</f>
+        <v>2.2291666666666665</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.2242990654205608</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.2226890756302522</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.215500945179584</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.2039249146757678</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.1904761904761907</v>
+      </c>
+      <c r="K15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.1769176387416049</v>
+      </c>
+      <c r="L15" s="9">
+        <f t="shared" si="6"/>
+        <v>2.1641633514654544</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9">
+        <f>E5/D5</f>
+        <v>2.1851851851851851</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16:L16" si="7">F5/E5</f>
+        <v>2.2203389830508473</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="7"/>
+        <v>2.2213740458015265</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="7"/>
+        <v>2.2096219931271479</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="shared" si="7"/>
+        <v>2.1944012441679628</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="7"/>
+        <v>2.179305457122608</v>
+      </c>
+      <c r="K16" s="9">
+        <f t="shared" si="7"/>
+        <v>2.1655284552845528</v>
+      </c>
+      <c r="L16" s="9">
+        <f t="shared" si="7"/>
+        <v>2.1533263252740653</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9">
+        <f>F6/E6</f>
+        <v>2.25</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" ref="G17:L17" si="8">G6/F6</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="8"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="shared" si="8"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="8"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="K17" s="9">
+        <f t="shared" si="8"/>
+        <v>2.1538461538461537</v>
+      </c>
+      <c r="L17" s="9">
+        <f t="shared" si="8"/>
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9">
+        <f t="shared" ref="G18:L21" si="9">G7/F7</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1538461538461537</v>
+      </c>
+      <c r="K18" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="L18" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1333333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1538461538461537</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" ref="J19:L19" si="10">J8/I8</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="K19" s="9">
+        <f t="shared" si="10"/>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="L19" s="9">
+        <f t="shared" si="10"/>
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="J20" s="9">
+        <f t="shared" ref="J20:L20" si="11">J9/I9</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="K20" s="9">
+        <f t="shared" si="11"/>
+        <v>2.125</v>
+      </c>
+      <c r="L20" s="9">
+        <f t="shared" si="11"/>
+        <v>2.1176470588235294</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9">
+        <f t="shared" ref="J21:L21" si="12">J10/I10</f>
+        <v>2.125</v>
+      </c>
+      <c r="K21" s="9">
+        <f t="shared" si="12"/>
+        <v>2.1176470588235294</v>
+      </c>
+      <c r="L21" s="9">
+        <f t="shared" si="12"/>
+        <v>2.1111111111111112</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9">
+        <f t="shared" ref="K22:L22" si="13">K11/J11</f>
+        <v>2.1111111111111112</v>
+      </c>
+      <c r="L22" s="9">
+        <f t="shared" si="13"/>
+        <v>2.1052631578947367</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Comparative Graphs and new excels
</commit_message>
<xml_diff>
--- a/2. Suma de enteros base DOS/SD-MTDeterminista1C.xlsx
+++ b/2. Suma de enteros base DOS/SD-MTDeterminista1C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34630\OneDrive\Escritorio\Universidad\4º\2º Cuatrimestre\TAC\P2MT\Practica_MT_TAC\2. Suma de enteros base DOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E697D-F748-4D9D-B97D-833A3B602A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604E4408-B35A-426E-BF35-DCA6ADACBDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F9F779F-0B5B-4B52-81CD-964E4560136B}"/>
   </bookViews>
@@ -1698,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A09BB4A-54DC-429E-B086-C294D4F51FFD}">
   <dimension ref="B2:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2272,7 +2272,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9">
-        <f t="shared" ref="G18:L21" si="9">G7/F7</f>
+        <f t="shared" ref="G18:L20" si="9">G7/F7</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="H18" s="9">

</xml_diff>